<commit_message>
update scripts, results, descriptions
</commit_message>
<xml_diff>
--- a/HJA_scripts/10_eo_data/environmental_covariate_descriptions.xlsx
+++ b/HJA_scripts/10_eo_data/environmental_covariate_descriptions.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1164" yWindow="2280" windowWidth="27636" windowHeight="16944"/>
+    <workbookView xWindow="1164" yWindow="2280" windowWidth="27636" windowHeight="16944" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="original vars" sheetId="1" r:id="rId1"/>
+    <sheet name="vars update" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'original vars'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="1417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="1536">
   <si>
     <t>SiteName</t>
   </si>
@@ -4287,6 +4288,363 @@
   </si>
   <si>
     <t>Same as SiteName?</t>
+  </si>
+  <si>
+    <t>ht30</t>
+  </si>
+  <si>
+    <t>gt4_r30</t>
+  </si>
+  <si>
+    <t>gt4_250</t>
+  </si>
+  <si>
+    <t>gt4_500</t>
+  </si>
+  <si>
+    <t>cut_r</t>
+  </si>
+  <si>
+    <t>cut_msk</t>
+  </si>
+  <si>
+    <t>cut_40msk</t>
+  </si>
+  <si>
+    <t>cut_r1k</t>
+  </si>
+  <si>
+    <t>cut_r500</t>
+  </si>
+  <si>
+    <t>cut_r250</t>
+  </si>
+  <si>
+    <t>cut40_r1k</t>
+  </si>
+  <si>
+    <t>cut40_r500</t>
+  </si>
+  <si>
+    <t>cut40_r250</t>
+  </si>
+  <si>
+    <t>be30</t>
+  </si>
+  <si>
+    <t>tri30</t>
+  </si>
+  <si>
+    <t>slope30</t>
+  </si>
+  <si>
+    <t>aspect30</t>
+  </si>
+  <si>
+    <t>Nss30</t>
+  </si>
+  <si>
+    <t>Ess30</t>
+  </si>
+  <si>
+    <t>twi30</t>
+  </si>
+  <si>
+    <t>tpi250</t>
+  </si>
+  <si>
+    <t>tpi500</t>
+  </si>
+  <si>
+    <t>tpi1k</t>
+  </si>
+  <si>
+    <t>DistStream</t>
+  </si>
+  <si>
+    <t>DistRoad</t>
+  </si>
+  <si>
+    <t>ndmi_stdDev_r100</t>
+  </si>
+  <si>
+    <t>ndmi_stdDev_r250</t>
+  </si>
+  <si>
+    <t>ndmi_stdDev_r500</t>
+  </si>
+  <si>
+    <t>nbr_stdDev_r100</t>
+  </si>
+  <si>
+    <t>nbr_stdDev_r250</t>
+  </si>
+  <si>
+    <t>nbr_stdDev_r500</t>
+  </si>
+  <si>
+    <t>ndvi_p5_r100</t>
+  </si>
+  <si>
+    <t>ndvi_p5_r250</t>
+  </si>
+  <si>
+    <t>ndvi_p5_r500</t>
+  </si>
+  <si>
+    <t>ndvi_p50_r100</t>
+  </si>
+  <si>
+    <t>ndvi_p50_r250</t>
+  </si>
+  <si>
+    <t>ndvi_p50_r500</t>
+  </si>
+  <si>
+    <t>ndvi_p95_r100</t>
+  </si>
+  <si>
+    <t>ndvi_p95_r250</t>
+  </si>
+  <si>
+    <t>ndvi_p95_r500</t>
+  </si>
+  <si>
+    <t>ndmi_p5_r100</t>
+  </si>
+  <si>
+    <t>ndmi_p5_r250</t>
+  </si>
+  <si>
+    <t>ndmi_p5_r500</t>
+  </si>
+  <si>
+    <t>ndmi_p50_r100</t>
+  </si>
+  <si>
+    <t>ndmi_p50_r250</t>
+  </si>
+  <si>
+    <t>ndmi_p50_r500</t>
+  </si>
+  <si>
+    <t>ndmi_p95_r100</t>
+  </si>
+  <si>
+    <t>ndmi_p95_r250</t>
+  </si>
+  <si>
+    <t>ndmi_p95_r500</t>
+  </si>
+  <si>
+    <t>LC08_045029_20180726_B1</t>
+  </si>
+  <si>
+    <t>LC08_045029_20180726_B3</t>
+  </si>
+  <si>
+    <t>LC08_045029_20180726_B4</t>
+  </si>
+  <si>
+    <t>LC08_045029_20180726_B5</t>
+  </si>
+  <si>
+    <t>LC08_045029_20180726_B7</t>
+  </si>
+  <si>
+    <t>LC08_045029_20180726_B10</t>
+  </si>
+  <si>
+    <t>meanT_annual</t>
+  </si>
+  <si>
+    <t>lg_DistStream</t>
+  </si>
+  <si>
+    <t>lg_DistRoad</t>
+  </si>
+  <si>
+    <t>lg_cover2m_max</t>
+  </si>
+  <si>
+    <t>lg_cover2m_4m</t>
+  </si>
+  <si>
+    <t>lg_cover4m_16m</t>
+  </si>
+  <si>
+    <t>Sample vars</t>
+  </si>
+  <si>
+    <t>Predictor vars</t>
+  </si>
+  <si>
+    <t>equivalent to be30 and elevation_m above</t>
+  </si>
+  <si>
+    <t>Previous vars</t>
+  </si>
+  <si>
+    <t>Area with or without disturbance (logging)</t>
+  </si>
+  <si>
+    <t>Area with or without disturbance (logging) in the last 40 years</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>proportion of area ever been logged (disturbed) within 500m radius</t>
+  </si>
+  <si>
+    <t>proportion of area ever been logged (disturbed) within 250m radius</t>
+  </si>
+  <si>
+    <t>proportion of area logged (disturbed) within last 40 years within 250m radius</t>
+  </si>
+  <si>
+    <t>proportion of area logged (disturbed) within last 40 years within 500m radius</t>
+  </si>
+  <si>
+    <t>proportion of area logged (disturbed) within last 40 years within 1km radius</t>
+  </si>
+  <si>
+    <t>proportion of area ever been logged (disturbed) within 1km radius</t>
+  </si>
+  <si>
+    <t>elevation in m derived from LIDAR (bare earth tif) at 30 m resolution (equivalent to elevation_m)</t>
+  </si>
+  <si>
+    <t>above logged log(x+0.001)</t>
+  </si>
+  <si>
+    <t>distance to road logged log(x+0.001)</t>
+  </si>
+  <si>
+    <t>distance to stream logged log(x+0.001)</t>
+  </si>
+  <si>
+    <t>standard deviation of annual NDMI, averaged over 250m radius</t>
+  </si>
+  <si>
+    <t>standard deviation of annual NDMI, averaged over 500m radius</t>
+  </si>
+  <si>
+    <t>standard deviation of annual NDMI, averaged over 100m radius = In Landsat 8, NDMI = (Band 5 – Band 6) / (Band 5 + Band 6)</t>
+  </si>
+  <si>
+    <t>standard deviation of annual NBR, averaged over 500m radius  = NBR = in Landsat 8 (Band 5 – Band 7) / (Band 5 + Band 7)</t>
+  </si>
+  <si>
+    <t>5% percentile of annual NDVI averaged over 100m radius.  Landsat 8, NDVI = (Band 5 – Band 4) / (Band 5 + Band 4).</t>
+  </si>
+  <si>
+    <t>5% percentile of annual NDVI averaged over 500m radius.  Landsat 8, NDVI = (Band 5 – Band 4) / (Band 5 + Band 4).</t>
+  </si>
+  <si>
+    <t>5% percentile of annual NDVI averaged over 250m radius.  Landsat 8, NDVI = (Band 5 – Band 4) / (Band 5 + Band 4).</t>
+  </si>
+  <si>
+    <t>median annual NDVI averaged over 100m radius</t>
+  </si>
+  <si>
+    <t>median annual NDVI averaged over 500m radius</t>
+  </si>
+  <si>
+    <t>median annual NDVI averaged over 250m radius</t>
+  </si>
+  <si>
+    <t>95% percentile annual NDVI over 100m radius</t>
+  </si>
+  <si>
+    <t>95% percentile annual NDVI over 500m radius</t>
+  </si>
+  <si>
+    <t>95% percentile annual NDVI over 250m radius</t>
+  </si>
+  <si>
+    <t>5% percentile annual NDMI over 100m radius</t>
+  </si>
+  <si>
+    <t>Landsat band B1 reflectance. 2018 07 26</t>
+  </si>
+  <si>
+    <t>Landsat band B10 reflectance. 2018 07 26</t>
+  </si>
+  <si>
+    <t>Landsat band B7 reflectance. 2018 07 26</t>
+  </si>
+  <si>
+    <t>Landsat band B5 reflectance. 2018 07 26</t>
+  </si>
+  <si>
+    <t>Landsat band B4 reflectance. 2018 07 26</t>
+  </si>
+  <si>
+    <t>Landsat band B3 reflectance. 2018 07 26</t>
+  </si>
+  <si>
+    <t>95% percentile NDMI over 100m radius</t>
+  </si>
+  <si>
+    <t>95% percentile NDMI over 500m radius</t>
+  </si>
+  <si>
+    <t>95% percentile NDMI over 250m radius</t>
+  </si>
+  <si>
+    <t>median NDMI over 100 m radisu</t>
+  </si>
+  <si>
+    <t>median NDMI over 250 m radius</t>
+  </si>
+  <si>
+    <t>median NDMI over 500 m radius</t>
+  </si>
+  <si>
+    <t>5% percentile annual NDMI over 250m radius</t>
+  </si>
+  <si>
+    <t>5% percentile annual NDMI over 500m radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard deviation of annual NBR over 250m radius </t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard deviation of annual NBR over 500m radius </t>
+  </si>
+  <si>
+    <t>be10 - be500 (equivalent to TPI above)</t>
+  </si>
+  <si>
+    <t>Proportion of vegetation cover over 4m, in 30 m radius</t>
+  </si>
+  <si>
+    <t>Proportion of vegetation cover over 4m, in 500 m radius</t>
+  </si>
+  <si>
+    <t>Proportion of vegetation cover over 4m, in 250 m radius</t>
+  </si>
+  <si>
+    <t>Topographic position index over 1km</t>
+  </si>
+  <si>
+    <t>Topographic position index over 500 m</t>
+  </si>
+  <si>
+    <t>Topographic position index over 250 m (central pixel - average elevation in surrounding window)</t>
+  </si>
+  <si>
+    <t># these vars produced as raster stack for training and prediction</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Years since last disturbance (areas without disturbance are NA) (ie 1925?- 2016)</t>
   </si>
 </sst>
 </file>
@@ -4317,7 +4675,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4348,6 +4706,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4361,7 +4725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4369,6 +4733,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4685,9 +5057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11908,4 +12280,1375 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="126.296875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="24.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>1495</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>1349</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>1482</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>1489</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>1488</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="7" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="7" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>1346</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="7" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>1529</v>
+      </c>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>1348</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1416</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="G60" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="G61" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="G62" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="G63" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="G64" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="G65" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="G66" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="G67" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="G68" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="G69" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E70" s="2"/>
+      <c r="G70" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="G71" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="G72" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>1377</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="G73" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="G74" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="G75" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="G76" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B77" s="7" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>1532</v>
+      </c>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B78" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="7" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>1530</v>
+      </c>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="G80" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="G81" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="G82" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="G83" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="G84" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="G85" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E86" s="2"/>
+      <c r="G86" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="G87" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E88" s="2"/>
+      <c r="G88" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="G89" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="G90" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>1407</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="G91" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="G92" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B93" s="7" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B94" s="7" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B95" s="7" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B96" s="7" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B97" s="7" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98" s="7" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99" s="7" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B100" s="7" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B101" s="7" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B102" s="7" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B103" s="7" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B104" s="7" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B105" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B106" s="7" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B107" s="7" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B108" s="7" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B109" s="7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B110" s="7" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B111" s="7" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B112" s="7" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B113" s="7" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B114" s="7" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B115" s="7" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B116" s="7" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B117" s="7" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B118" s="7" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B119" s="7" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B120" s="7" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B121" s="7" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B122" s="7" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>